<commit_message>
integrated alternatives to death sellships bug testing
</commit_message>
<xml_diff>
--- a/getting_a_job/relation-faction_values.xlsx
+++ b/getting_a_job/relation-faction_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Steam\steamapps\common\X4 Foundations\extension files\Mods\getting_a_job\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Steam\steamapps\common\X4 Foundations\extensions\getting_a_job\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A758FED-DA36-4F9E-A97B-67F8198EF948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DD7E65-1D27-4B78-A5D8-C8F5A1EF874C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12285" yWindow="60" windowWidth="16620" windowHeight="15345" xr2:uid="{DCB5B74E-3098-4241-89CB-2C397A9248D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCB5B74E-3098-4241-89CB-2C397A9248D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,417 +224,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1075,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3B2B57-4486-4097-ABDA-82D973D1485E}">
-  <dimension ref="H8:X43"/>
+  <dimension ref="H4:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,6 +684,34 @@
     <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>1.58489319246111E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>1.5924250000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f>M7-M5</f>
+        <v>1.1649223252696572E-12</v>
+      </c>
+    </row>
+    <row r="7" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <f>10^(J7 / 10) / $N$7</f>
+        <v>1.5924250001164923E-2</v>
+      </c>
+      <c r="N7">
+        <v>995.27022769999996</v>
+      </c>
+    </row>
     <row r="8" spans="8:24" x14ac:dyDescent="0.25">
       <c r="H8">
         <v>0</v>
@@ -1104,8 +722,11 @@
       <c r="J8">
         <v>0</v>
       </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
       <c r="M8">
-        <v>1.2589254117947</v>
+        <v>1.2589999999999999</v>
       </c>
     </row>
     <row r="9" spans="8:24" x14ac:dyDescent="0.25">
@@ -1118,9 +739,8 @@
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="L9" s="3">
-        <f t="shared" ref="L9:L17" si="0">ROUNDDOWN(M9,6)</f>
-        <v>1.258E-3</v>
+      <c r="L9" s="6">
+        <v>6.4000000000000005E-4</v>
       </c>
       <c r="M9" s="4">
         <v>1.25892541179E-3</v>
@@ -1136,13 +756,12 @@
       <c r="J10">
         <v>2</v>
       </c>
-      <c r="L10" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5839999999999999E-3</v>
+      <c r="L10" s="6">
+        <v>1.2800000000000001E-3</v>
       </c>
       <c r="M10" s="4">
         <f>M9*$M$8</f>
-        <v>1.5848931924565381E-3</v>
+        <v>1.58498709344361E-3</v>
       </c>
       <c r="O10" t="s">
         <v>42</v>
@@ -1182,13 +801,12 @@
       <c r="J11">
         <v>3</v>
       </c>
-      <c r="L11" s="3">
-        <f t="shared" si="0"/>
-        <v>1.9949999999999998E-3</v>
+      <c r="L11" s="6">
+        <v>1.92E-3</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" ref="M11:M38" si="1">M10*$M$8</f>
-        <v>1.995262314963964E-3</v>
+        <f t="shared" ref="M11:M38" si="0">M10*$M$8</f>
+        <v>1.995498750645505E-3</v>
       </c>
       <c r="O11" t="s">
         <v>7</v>
@@ -1222,13 +840,12 @@
       <c r="J12">
         <v>4</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="6">
+        <v>2.5600000000000002E-3</v>
+      </c>
+      <c r="M12" s="4">
         <f t="shared" si="0"/>
-        <v>2.5110000000000002E-3</v>
-      </c>
-      <c r="M12" s="4">
-        <f t="shared" si="1"/>
-        <v>2.5118864315044546E-3</v>
+        <v>2.5123329270626904E-3</v>
       </c>
       <c r="O12" t="s">
         <v>9</v>
@@ -1262,14 +879,10 @@
       <c r="J13">
         <v>5</v>
       </c>
-      <c r="L13" s="3">
-        <f t="shared" si="0"/>
-        <v>3.1619999999999999E-3</v>
-      </c>
-      <c r="M13" s="4">
-        <f t="shared" si="1"/>
-        <v>3.162277660163265E-3</v>
-      </c>
+      <c r="L13" s="6">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="M13" s="4"/>
       <c r="O13" t="s">
         <v>10</v>
       </c>
@@ -1294,12 +907,12 @@
         <v>6</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="0"/>
-        <v>3.9810000000000002E-3</v>
-      </c>
-      <c r="M14" s="4">
-        <f t="shared" si="1"/>
-        <v>3.9810717055302185E-3</v>
+        <f t="shared" ref="L9:L17" si="1">ROUNDDOWN(M14,6)</f>
+        <v>3.999E-3</v>
+      </c>
+      <c r="M14">
+        <f>10^(J14 / 10) / $N$7</f>
+        <v>3.9999907509892579E-3</v>
       </c>
       <c r="O14" t="s">
         <v>11</v>
@@ -1328,12 +941,12 @@
         <v>7</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="0"/>
-        <v>5.0109999999999998E-3</v>
-      </c>
-      <c r="M15" s="4">
         <f t="shared" si="1"/>
-        <v>5.0118723362688588E-3</v>
+        <v>5.0350000000000004E-3</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15:M38" si="2">10^(J15 / 10) / $N$7</f>
+        <v>5.0356900033620118E-3</v>
       </c>
       <c r="O15" t="s">
         <v>12</v>
@@ -1362,12 +975,12 @@
         <v>8</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="0"/>
-        <v>6.3090000000000004E-3</v>
-      </c>
-      <c r="M16" s="4">
         <f t="shared" si="1"/>
-        <v>6.3095734447997385E-3</v>
+        <v>6.339E-3</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>6.3395581111502933E-3</v>
       </c>
       <c r="O16" t="s">
         <v>13</v>
@@ -1402,12 +1015,12 @@
         <v>9</v>
       </c>
       <c r="L17" s="3">
-        <f t="shared" si="0"/>
-        <v>7.9430000000000004E-3</v>
-      </c>
-      <c r="M17" s="4">
         <f t="shared" si="1"/>
-        <v>7.943282347243414E-3</v>
+        <v>7.9810000000000002E-3</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>7.9810308056729364E-3</v>
       </c>
       <c r="O17" t="s">
         <v>14</v>
@@ -1439,12 +1052,12 @@
         <v>10</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" ref="L18:L27" si="2">ROUNDDOWN(M18,5)</f>
-        <v>0.01</v>
-      </c>
-      <c r="M18" s="4">
-        <f t="shared" si="1"/>
-        <v>1.0000000000004986E-2</v>
+        <f t="shared" ref="L18:L27" si="3">ROUNDDOWN(M18,5)</f>
+        <v>1.004E-2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>1.0047522493573732E-2</v>
       </c>
       <c r="O18" t="s">
         <v>15</v>
@@ -1479,12 +1092,12 @@
         <v>11</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="2"/>
-        <v>1.2579999999999999E-2</v>
-      </c>
-      <c r="M19" s="4">
-        <f t="shared" si="1"/>
-        <v>1.2589254117953277E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.264E-2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>1.2649081392733477E-2</v>
       </c>
       <c r="O19" t="s">
         <v>16</v>
@@ -1519,12 +1132,12 @@
         <v>12</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="2"/>
-        <v>1.584E-2</v>
-      </c>
-      <c r="M20" s="4">
-        <f t="shared" si="1"/>
-        <v>1.5848931924632451E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.592E-2</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>1.5924250001164923E-2</v>
       </c>
       <c r="O20" t="s">
         <v>17</v>
@@ -1562,12 +1175,12 @@
         <v>13</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="2"/>
-        <v>1.9949999999999999E-2</v>
-      </c>
-      <c r="M21" s="4">
-        <f t="shared" si="1"/>
-        <v>1.9952623149724076E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.0039999999999999E-2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>2.0047442990229824E-2</v>
       </c>
       <c r="O21" t="s">
         <v>18</v>
@@ -1599,12 +1212,12 @@
         <v>14</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="2"/>
-        <v>2.511E-2</v>
-      </c>
-      <c r="M22" s="4">
-        <f t="shared" si="1"/>
-        <v>2.5118864315150848E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.5229999999999999E-2</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="2"/>
+        <v>2.5238235421895159E-2</v>
       </c>
       <c r="O22" t="s">
         <v>19</v>
@@ -1639,12 +1252,11 @@
         <v>15</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="2"/>
-        <v>3.1620000000000002E-2</v>
-      </c>
-      <c r="M23" s="4">
-        <f t="shared" si="1"/>
-        <v>3.1622776601766475E-2</v>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="2"/>
+        <v>3.1773055921467515E-2</v>
       </c>
       <c r="O23" t="s">
         <v>20</v>
@@ -1670,12 +1282,12 @@
         <v>16</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="2"/>
-        <v>3.9809999999999998E-2</v>
-      </c>
-      <c r="M24" s="4">
-        <f t="shared" si="1"/>
-        <v>3.9810717055470665E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.9989999999999998E-2</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>3.9999907509892609E-2</v>
       </c>
       <c r="O24" t="s">
         <v>21</v>
@@ -1707,12 +1319,12 @@
         <v>17</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="2"/>
-        <v>5.0110000000000002E-2</v>
-      </c>
-      <c r="M25" s="4">
-        <f t="shared" si="1"/>
-        <v>5.0118723362900693E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.0349999999999999E-2</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="2"/>
+        <v>5.0356900033620124E-2</v>
       </c>
       <c r="O25" t="s">
         <v>23</v>
@@ -1735,12 +1347,12 @@
         <v>18</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="2"/>
-        <v>6.3089999999999993E-2</v>
-      </c>
-      <c r="M26" s="4">
-        <f t="shared" si="1"/>
-        <v>6.3095734448264398E-2</v>
+        <f t="shared" si="3"/>
+        <v>6.3390000000000002E-2</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="2"/>
+        <v>6.3395581111502952E-2</v>
       </c>
       <c r="O26" t="s">
         <v>24</v>
@@ -1775,12 +1387,12 @@
         <v>19</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="2"/>
-        <v>7.9430000000000001E-2</v>
-      </c>
-      <c r="M27" s="4">
-        <f t="shared" si="1"/>
-        <v>7.9432823472770295E-2</v>
+        <f t="shared" si="3"/>
+        <v>7.9810000000000006E-2</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="2"/>
+        <v>7.9810308056729382E-2</v>
       </c>
       <c r="O27" t="s">
         <v>25</v>
@@ -1812,12 +1424,11 @@
         <v>20</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" ref="L28:L37" si="3">ROUNDDOWN(M28,4)</f>
         <v>0.1</v>
       </c>
-      <c r="M28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.10000000000047306</v>
+      <c r="M28">
+        <f t="shared" si="2"/>
+        <v>0.10047522493573732</v>
       </c>
       <c r="O28" t="s">
         <v>26</v>
@@ -1852,12 +1463,12 @@
         <v>21</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="3"/>
-        <v>0.1258</v>
-      </c>
-      <c r="M29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12589254118006554</v>
+        <f t="shared" ref="L28:L37" si="4">ROUNDDOWN(M29,4)</f>
+        <v>0.12640000000000001</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>0.12649081392733474</v>
       </c>
       <c r="O29" t="s">
         <v>27</v>
@@ -1883,12 +1494,12 @@
         <v>22</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="3"/>
-        <v>0.15840000000000001</v>
-      </c>
-      <c r="M30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.15848931924699525</v>
+        <f t="shared" si="4"/>
+        <v>0.15920000000000001</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="2"/>
+        <v>0.15924250001164938</v>
       </c>
       <c r="O30" t="s">
         <v>28</v>
@@ -1914,12 +1525,12 @@
         <v>23</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="3"/>
-        <v>0.19950000000000001</v>
-      </c>
-      <c r="M31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.19952623149808515</v>
+        <f t="shared" si="4"/>
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="2"/>
+        <v>0.20047442990229822</v>
       </c>
       <c r="O31" t="s">
         <v>29</v>
@@ -1951,12 +1562,12 @@
         <v>24</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="3"/>
-        <v>0.25109999999999999</v>
-      </c>
-      <c r="M32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2511886431525715</v>
+        <f t="shared" si="4"/>
+        <v>0.25230000000000002</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="2"/>
+        <v>0.25238235421895167</v>
       </c>
       <c r="O32" t="s">
         <v>30</v>
@@ -1991,12 +1602,11 @@
         <v>25</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="3"/>
-        <v>0.31619999999999998</v>
-      </c>
-      <c r="M33" s="4">
-        <f t="shared" si="1"/>
-        <v>0.31622776601900304</v>
+        <v>0.32</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="2"/>
+        <v>0.31773055921467536</v>
       </c>
       <c r="O33" t="s">
         <v>31</v>
@@ -2031,12 +1641,12 @@
         <v>26</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="3"/>
-        <v>0.39810000000000001</v>
-      </c>
-      <c r="M34" s="4">
-        <f t="shared" si="1"/>
-        <v>0.39810717055639144</v>
+        <f t="shared" si="4"/>
+        <v>0.39989999999999998</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="2"/>
+        <v>0.39999907509892613</v>
       </c>
       <c r="O34" t="s">
         <v>32</v>
@@ -2068,12 +1678,12 @@
         <v>27</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="3"/>
-        <v>0.50109999999999999</v>
-      </c>
-      <c r="M35" s="4">
-        <f t="shared" si="1"/>
-        <v>0.50118723363112794</v>
+        <f t="shared" si="4"/>
+        <v>0.50349999999999995</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="2"/>
+        <v>0.50356900033620156</v>
       </c>
       <c r="O35" t="s">
         <v>33</v>
@@ -2105,12 +1715,12 @@
         <v>28</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="3"/>
-        <v>0.63090000000000002</v>
-      </c>
-      <c r="M36" s="4">
-        <f t="shared" si="1"/>
-        <v>0.63095734448531426</v>
+        <f t="shared" si="4"/>
+        <v>0.63390000000000002</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="2"/>
+        <v>0.63395581111502919</v>
       </c>
       <c r="O36" t="s">
         <v>34</v>
@@ -2142,12 +1752,12 @@
         <v>29</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="3"/>
-        <v>0.79430000000000001</v>
-      </c>
-      <c r="M37" s="4">
-        <f t="shared" si="1"/>
-        <v>0.79432823473106462</v>
+        <f t="shared" si="4"/>
+        <v>0.79810000000000003</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="2"/>
+        <v>0.79810308056729395</v>
       </c>
       <c r="O37" t="s">
         <v>35</v>
@@ -2182,12 +1792,11 @@
         <v>30</v>
       </c>
       <c r="L38" s="5">
-        <f>ROUNDDOWN(M38,3)</f>
         <v>1</v>
       </c>
-      <c r="M38" s="4">
-        <f t="shared" si="1"/>
-        <v>1.0000000000089626</v>
+      <c r="M38">
+        <f t="shared" si="2"/>
+        <v>1.0047522493573733</v>
       </c>
       <c r="O38" t="s">
         <v>40</v>
@@ -2287,38 +1896,38 @@
       <sortCondition ref="Q10:Q59"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M44">
-    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M45">
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46">
-    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M47">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M48">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M51:M53">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10 O44:O51">
+    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11:O42 L92">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10 O44:O51">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>